<commit_message>
Added more into the theory section. Specifically tables for fermions and bosons. Also added pdg as a reference.
</commit_message>
<xml_diff>
--- a/Dissertation Writing Schedule.xlsx
+++ b/Dissertation Writing Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eparrish/Work/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{383D7CF5-D5F8-534A-B5DA-6961781B9EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FAF84F-5780-EA4F-BFA3-4C3F3821EB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19980" windowHeight="12020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23340" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TASKS" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>MY TASKS</t>
   </si>
@@ -61,9 +61,6 @@
     <t>% COMPLETE</t>
   </si>
   <si>
-    <t>Dissertattion Writing Schedule</t>
-  </si>
-  <si>
     <t>Standard Model</t>
   </si>
   <si>
@@ -97,13 +94,40 @@
     <t>Results</t>
   </si>
   <si>
-    <t>Conclusion</t>
-  </si>
-  <si>
     <t>Acknowledgements</t>
   </si>
   <si>
-    <t>77/28/22</t>
+    <t>Dissertation Writing Schedule</t>
+  </si>
+  <si>
+    <t>Intro/Conclusion</t>
+  </si>
+  <si>
+    <t>Sarah visits - 7/22-26</t>
+  </si>
+  <si>
+    <t>DGD 8/8</t>
+  </si>
+  <si>
+    <t>WFF 8/19-21</t>
+  </si>
+  <si>
+    <t>Anniversary  8/27</t>
+  </si>
+  <si>
+    <t>Restaurant</t>
+  </si>
+  <si>
+    <t>Weekends off</t>
+  </si>
+  <si>
+    <t>8/17 - 8/19</t>
+  </si>
+  <si>
+    <t>8/26 - 8/29</t>
+  </si>
+  <si>
+    <t>8/5-8/8</t>
   </si>
 </sst>
 </file>
@@ -194,7 +218,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -211,6 +235,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -235,7 +300,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -274,6 +339,24 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -286,38 +369,6 @@
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="12">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -372,6 +423,38 @@
         <color theme="0"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="0"/>
       </font>
       <fill>
         <patternFill>
@@ -504,15 +587,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tasks" displayName="Tasks" ref="B2:G15" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowCellStyle="Heading 1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tasks" displayName="Tasks" ref="B2:G15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" headerRowCellStyle="Heading 1">
   <autoFilter ref="B2:G15" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="MY TASKS" dataDxfId="7" dataCellStyle="Table Text"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="START DATE" dataDxfId="6" dataCellStyle="Date"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="DUE DATE" dataDxfId="5" dataCellStyle="Date"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="% COMPLETE" dataDxfId="4" dataCellStyle="Percent"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="DONE" dataDxfId="3" dataCellStyle="Done"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="NOTES" dataDxfId="2" dataCellStyle="Table Text"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="MY TASKS" dataDxfId="5" dataCellStyle="Table Text"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="START DATE" dataDxfId="4" dataCellStyle="Date"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="DUE DATE" dataDxfId="3" dataCellStyle="Date"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="% COMPLETE" dataDxfId="2" dataCellStyle="Percent"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="DONE" dataDxfId="1" dataCellStyle="Done"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="NOTES" dataDxfId="0" dataCellStyle="Table Text"/>
   </tableColumns>
   <tableStyleInfo name="Task List" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -730,10 +813,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G15"/>
+  <dimension ref="B1:L15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -749,9 +832,9 @@
     <col min="9" max="16384" width="8.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -759,7 +842,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -778,10 +861,16 @@
       <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="8">
         <v>44756</v>
@@ -794,10 +883,16 @@
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I3" s="17">
+        <v>44762</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="8">
         <v>44762</v>
@@ -810,10 +905,16 @@
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="8">
         <v>44766</v>
@@ -826,10 +927,14 @@
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J5" s="14"/>
+      <c r="L5" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="8">
         <v>44768</v>
@@ -843,15 +948,15 @@
       <c r="F6" s="12"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="8">
         <v>44769</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>20</v>
+      <c r="D7" s="8">
+        <v>44770</v>
       </c>
       <c r="E7" s="11">
         <v>0</v>
@@ -859,12 +964,12 @@
       <c r="F7" s="12"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="8">
-        <v>44768</v>
+        <v>44770</v>
       </c>
       <c r="D8" s="8">
         <v>44773</v>
@@ -875,9 +980,9 @@
       <c r="F8" s="12"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="8">
         <v>44774</v>
@@ -891,9 +996,9 @@
       <c r="F9" s="12"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="8">
         <v>44781</v>
@@ -906,10 +1011,13 @@
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J10" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="8">
         <v>44785</v>
@@ -923,9 +1031,9 @@
       <c r="F11" s="12"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="8">
         <v>44792</v>
@@ -938,10 +1046,13 @@
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J12" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="8">
         <v>44797</v>
@@ -954,10 +1065,13 @@
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J13" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C14" s="8">
         <v>44802</v>
@@ -971,9 +1085,9 @@
       <c r="F14" s="12"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" s="8">
         <v>44805</v>
@@ -989,6 +1103,9 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="J4:J5"/>
+  </mergeCells>
   <conditionalFormatting sqref="E3:E15">
     <cfRule type="dataBar" priority="6">
       <dataBar>

</xml_diff>